<commit_message>
included Gryffin for comparison study
</commit_message>
<xml_diff>
--- a/case_studies/case_study_pwas/z_comparisonStudy/crossed_barrel/z_results/cpu_time_analysis.xlsx
+++ b/case_studies/case_study_pwas/z_comparisonStudy/crossed_barrel/z_results/cpu_time_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mengjia\Desktop\IMT\z-Research\a_on_going_project\MILP_IC\Rxn opt benchmark\z_olympus_code\olympus\case_studies\case_study_pwas\z_comparisonStudy\crossed_barrel\z_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemanchesterac-my.sharepoint.com/personal/mengjia_zhu_manchester_ac_uk/Documents/Desktop/UoM/z_research/zzz_GitHub repo/olympus/case_studies/case_study_pwas/z_comparisonStudy/crossed_barrel/z_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C104F2-36E6-423B-BACD-06F15B92F5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{00C104F2-36E6-423B-BACD-06F15B92F5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FA08D05-EA81-4DE5-9963-B18FD9C7FB4A}"/>
   <bookViews>
-    <workbookView xWindow="-14385" yWindow="-18360" windowWidth="29040" windowHeight="17520" xr2:uid="{D5C986B5-AE09-414B-A63B-0071D8A10DEA}"/>
+    <workbookView xWindow="-13290" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D5C986B5-AE09-414B-A63B-0071D8A10DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="cpu time" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Random</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>Gryffin</t>
   </si>
 </sst>
 </file>
@@ -438,15 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D259BE6F-E20E-4E3C-B4AE-68FEA59E9920}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +474,11 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,8 +506,11 @@
       <c r="I2">
         <v>217.828125</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>89.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -529,8 +538,11 @@
       <c r="I3">
         <v>208.015625</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>70.03125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -558,8 +570,11 @@
       <c r="I4">
         <v>213.984375</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>86.3125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -587,8 +602,11 @@
       <c r="I5">
         <v>211.109375</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>54.109375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -616,8 +634,11 @@
       <c r="I6">
         <v>201.828125</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>46.328125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -645,8 +666,11 @@
       <c r="I7">
         <v>225.515625</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>114.546875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -674,8 +698,11 @@
       <c r="I8">
         <v>203.265625</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>116.203125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -703,8 +730,11 @@
       <c r="I9">
         <v>211.296875</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>159.015625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -732,8 +762,11 @@
       <c r="I10">
         <v>224.328125</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>156.515625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -761,8 +794,11 @@
       <c r="I11">
         <v>207.46875</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>113.875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -790,8 +826,11 @@
       <c r="I12">
         <v>210.59375</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>675.6875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -819,8 +858,11 @@
       <c r="I13">
         <v>312.453125</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>169.890625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -848,8 +890,11 @@
       <c r="I14">
         <v>226.46875</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>82.765625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -877,8 +922,11 @@
       <c r="I15">
         <v>212.6875</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>140.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -906,8 +954,11 @@
       <c r="I16">
         <v>199.078125</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>108.171875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -935,8 +986,11 @@
       <c r="I17">
         <v>205.234375</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>105.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -964,8 +1018,11 @@
       <c r="I18">
         <v>212.171875</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>121.421875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -993,8 +1050,11 @@
       <c r="I19">
         <v>195.65625</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>142.90625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1022,8 +1082,11 @@
       <c r="I20">
         <v>216.515625</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>158.65625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1051,8 +1114,11 @@
       <c r="I21">
         <v>199.265625</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>173.234375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1080,8 +1146,11 @@
       <c r="I22">
         <v>208.921875</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>158.796875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1109,8 +1178,11 @@
       <c r="I23">
         <v>202.546875</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>149.296875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1138,8 +1210,11 @@
       <c r="I24">
         <v>215.59375</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>166.015625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1167,8 +1242,11 @@
       <c r="I25">
         <v>205.0625</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>155.953125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1196,8 +1274,11 @@
       <c r="I26">
         <v>201.28125</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>153.765625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1225,8 +1306,11 @@
       <c r="I27">
         <v>209.75</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>158.421875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1254,8 +1338,11 @@
       <c r="I28">
         <v>208.234375</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>153.0625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1283,8 +1370,11 @@
       <c r="I29">
         <v>214.5625</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>152.109375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1312,8 +1402,11 @@
       <c r="I30">
         <v>197.515625</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>168.703125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1341,13 +1434,16 @@
       <c r="I31">
         <v>209.421875</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>150.234375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" ref="B33:I33" si="0">AVERAGE(B2:B31)</f>
+        <f t="shared" ref="B33:J33" si="0">AVERAGE(B2:B31)</f>
         <v>1.8489583333333333</v>
       </c>
       <c r="C33" s="1">
@@ -1378,8 +1474,12 @@
         <f t="shared" si="0"/>
         <v>212.921875</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>148.37604166666668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1412,8 +1512,12 @@
         <v>2.5206038534286859</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34" si="4">_xlfn.STDEV.S(I2:I31)</f>
+        <f t="shared" ref="I34:J34" si="4">_xlfn.STDEV.S(I2:I31)</f>
         <v>20.381378163292325</v>
+      </c>
+      <c r="J34" s="1">
+        <f>_xlfn.STDEV.S(J2:J31)</f>
+        <v>105.89257642221391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>